<commit_message>
Changes in template.  Renamed to networktest
</commit_message>
<xml_diff>
--- a/config/template.xlsx
+++ b/config/template.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ausdrillltd.sharepoint.com/sites/InnovationandTechnologyTeam/Shared Documents/General/0.A&amp;MT/WoC/WoC-FAT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K\Documents\networktest\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{42C45D93-E78C-470B-A3E4-5D51921F44A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B53410B2-BC26-4235-8CDE-6E39C0A96FB4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2514A02E-7F76-47B6-AC16-78830D4353BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F2D3511-4593-4228-B827-829CFE5D647D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F2D3511-4593-4228-B827-829CFE5D647D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$62</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$10</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,19 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Testing Parameters</t>
-  </si>
-  <si>
-    <t>Equipment Description: WoC-1000-WiFi4</t>
-  </si>
-  <si>
-    <t>TCP Total Throughput (Mb/s)</t>
-  </si>
-  <si>
-    <t>UDP Total Throughput (Mb/s)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Jitter (ms)</t>
   </si>
@@ -68,28 +60,16 @@
     <t>Time of Test:</t>
   </si>
   <si>
-    <t xml:space="preserve">Equipment Serial Number: </t>
-  </si>
-  <si>
     <t>TCP Throughput:</t>
   </si>
   <si>
-    <t xml:space="preserve">Equipment MAC Address: </t>
-  </si>
-  <si>
     <t>UDP Throughput:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IP Address: </t>
   </si>
   <si>
     <t>Network Port:</t>
   </si>
   <si>
     <t>Location:</t>
-  </si>
-  <si>
-    <t>wifi stuff…</t>
   </si>
   <si>
     <t>Engineer:</t>
@@ -111,6 +91,12 @@
   </si>
   <si>
     <t>Functional Network Test</t>
+  </si>
+  <si>
+    <t>TCP (Mb/s)</t>
+  </si>
+  <si>
+    <t>UDP (Mb/s)</t>
   </si>
 </sst>
 </file>
@@ -160,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,83 +158,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -273,114 +182,74 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -398,6 +267,85 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>828674</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>450193</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>733424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2043E050-B968-4B22-B9D5-B05F57DD3F1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6972299" y="133349"/>
+          <a:ext cx="3183869" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -697,799 +645,932 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1CBCEC-DFB6-416D-A969-08EEC6C4034F}">
-  <dimension ref="A1:O50"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="8" customWidth="1"/>
-    <col min="3" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="35.140625" style="5" customWidth="1"/>
-    <col min="9" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="9.140625" style="24"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="6" customWidth="1"/>
+    <col min="3" max="7" width="9.140625" style="6"/>
+    <col min="8" max="8" width="35.140625" style="4" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>24</v>
+    <row r="1" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>16</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="23"/>
-      <c r="N1" s="12" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="13"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="16" t="s">
+      <c r="G2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="H2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="I2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="16" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="N2" s="13" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="13"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="N3" s="13" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="13"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="J9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="25"/>
-      <c r="N4" s="13" t="s">
+      <c r="K9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="13"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="N5" s="13" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="13"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="N6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="13"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="26"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="28"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="32"/>
+      <c r="H12" s="15"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="28"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="32"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="28"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="17"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="31"/>
+      <c r="H15" s="17"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="7"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="31"/>
+      <c r="H16" s="17"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="28"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="31"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="28"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="31"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="28"/>
+      <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="31"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="28"/>
+      <c r="L19" s="11"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="32"/>
+      <c r="H20" s="15"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="28"/>
+      <c r="L20" s="11"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="31"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="28"/>
+      <c r="L21" s="11"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="7"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="32"/>
+      <c r="H22" s="15"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="28"/>
+      <c r="L22" s="11"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="31"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="28"/>
+      <c r="L23" s="11"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="32"/>
+      <c r="H24" s="15"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="28"/>
+      <c r="L24" s="11"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="32"/>
+      <c r="H25" s="15"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="28"/>
+      <c r="L25" s="11"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="32"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="28"/>
+      <c r="L26" s="11"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="32"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="28"/>
+      <c r="L27" s="11"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="7"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="32"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="28"/>
+      <c r="L28" s="11"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="7"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="32"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="28"/>
+      <c r="L29" s="11"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="32"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="28"/>
+      <c r="L30" s="11"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="7"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="32"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="28"/>
+      <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="7"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="32"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="28"/>
+      <c r="L32" s="11"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="7"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="32"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-      <c r="L33" s="28"/>
+      <c r="L33" s="11"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="7"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="32"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="28"/>
+      <c r="L34" s="11"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="7"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="32"/>
+      <c r="H35" s="12"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" s="28"/>
+      <c r="L35" s="11"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="7"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="32"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="28"/>
+      <c r="L36" s="11"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="7"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="32"/>
+      <c r="H37" s="12"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="28"/>
+      <c r="L37" s="11"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="7"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="32"/>
+      <c r="H38" s="12"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="L38" s="28"/>
+      <c r="L38" s="11"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="7"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="32"/>
+      <c r="H39" s="12"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="L39" s="28"/>
+      <c r="L39" s="11"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="7"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="32"/>
+      <c r="H40" s="12"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="L40" s="28"/>
+      <c r="L40" s="11"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="7"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="32"/>
+      <c r="H41" s="12"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="L41" s="28"/>
+      <c r="L41" s="11"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="7"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="32"/>
+      <c r="H42" s="12"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="L42" s="28"/>
+      <c r="L42" s="11"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="B43" s="7"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="32"/>
+      <c r="H43" s="12"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="28"/>
+      <c r="L43" s="11"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" s="7"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="32"/>
+      <c r="H44" s="12"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="28"/>
+      <c r="L44" s="11"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="7"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="32"/>
+      <c r="H45" s="12"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="28"/>
+      <c r="L45" s="11"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="7"/>
+      <c r="B46" s="5"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="32"/>
+      <c r="H46" s="12"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="28"/>
+      <c r="L46" s="11"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="7"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="32"/>
+      <c r="H47" s="12"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="28"/>
+      <c r="L47" s="11"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="7"/>
+      <c r="B48" s="5"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="32"/>
+      <c r="H48" s="12"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="28"/>
+      <c r="L48" s="11"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="7"/>
+      <c r="B49" s="5"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="32"/>
+      <c r="H49" s="12"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="L49" s="28"/>
+      <c r="L49" s="11"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="7"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="32"/>
+      <c r="H50" s="12"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="28"/>
+      <c r="L50" s="11"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A9:G9"/>
+  <mergeCells count="12">
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="I2:K8"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
-    <mergeCell ref="C2:C8"/>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="G2:G8"/>
-    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="H2:H10"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="G2:G9"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="85" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>